<commit_message>
replaced missing topics in risk assessment & management
</commit_message>
<xml_diff>
--- a/app/source_data/Maturity_Assessment_Data.xlsx
+++ b/app/source_data/Maturity_Assessment_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\maturity-assessment-2\app\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1434B1BF-DE0E-4E8D-AE39-4D8A2F7EEE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521374AA-4467-4945-A125-97A0F2B4C51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="735" windowWidth="42600" windowHeight="13050" tabRatio="822" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="1305" windowWidth="25995" windowHeight="13050" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enhanced Framework" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Acronyms" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Dimension Theme Topic Descrip'!$J$1:$J$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Dimension Theme Topic Descrip'!$J$1:$J$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="1730">
   <si>
     <t>Dimension</t>
   </si>
@@ -6873,6 +6873,114 @@
   </si>
   <si>
     <t>All technologies used to create, process, store, transmit, and retrieve digital information</t>
+  </si>
+  <si>
+    <t>Risk monitoring and trending analysis</t>
+  </si>
+  <si>
+    <t>Structured analysis of time‑series indicators (incidents, losses, KRIs, capacity headroom, supplier findings) to detect deterioration or improvements, using thresholds, run charts and statistical tests to guide action.</t>
+  </si>
+  <si>
+    <t>• Backwards‑looking MI without trend context; slow reactions
+• Volatility mistaken for trend; false alarms or complacency
+• Findings not linked to ownership, actions or outcomes</t>
+  </si>
+  <si>
+    <t>• Earlier recognition of emerging problems; fewer severe incidents
+• Noise reduced through statistical methods; better focus
+• Clear accountability and evidence of improvement</t>
+  </si>
+  <si>
+    <t>• Monthly trend pack with standard charts and commentary
+• Ownership and action fields; simple thresholds
+• Manual reconciliation with incident and change calendars</t>
+  </si>
+  <si>
+    <t>• Automated trend detection (CUSUM, EWMA); seasonality adjustments
+• Correlation with change/events; service/vendor drill‑downs
+• Benefits realisation tracked against actions/funding</t>
+  </si>
+  <si>
+    <t>• Trend dashboards with methods documented; alert history and outcomes
+• Action logs with effect on trends; reduced false alarms
+• Governance minutes referencing trend analyses</t>
+  </si>
+  <si>
+    <t>ISO 22301 performance/measurement; BCBS PSMOR (metrics &amp; monitoring); FCA PS21/3 (Board MI)</t>
+  </si>
+  <si>
+    <t>Threshold breach escalation playbooks</t>
+  </si>
+  <si>
+    <t>Pre‑agreed responses when KRIs or tolerance headroom cross thresholds: who is paged, what analysis is done, decision options (halt change, add capacity, customer comms), and when to declare an incident.</t>
+  </si>
+  <si>
+    <t>• Breach emails ignored; unclear ownership; slow or wrong responses
+• Repeated breaches with no root‑cause or structural fix
+• Regulators challenge why tolerances/KRIs exist if breaches not acted on</t>
+  </si>
+  <si>
+    <t>• Faster, consistent actions reduce customer harm and breach duration
+• Clear audit trail from breach to decision and outcome
+• Learning loop strengthens thresholds and controls</t>
+  </si>
+  <si>
+    <t>• Runbooks per KRI/tolerance with roles, time targets and decision trees
+• Paging lists and comms templates; manual evidence capture
+• Periodic simulations/table‑tops of breach scenarios</t>
+  </si>
+  <si>
+    <t>• Automated trigger→runbook execution via ChatOps/ITSM; guardrails
+• Integrated root‑cause prompts and structural fix catalogues
+• MI on time‑to‑action, recurrence and effect on outcomes</t>
+  </si>
+  <si>
+    <t>• Breach logs linked to runbooks and decisions
+• Evidence of structural fixes, not just temporary mitigations
+• Improved breach metrics over time with governance reviews</t>
+  </si>
+  <si>
+    <t>FCA PS21/3 (tolerances &amp; MI), ISO 22301 (response &amp; performance), BCBS PSMOR (risk response), DORA (monitoring/reporting)</t>
+  </si>
+  <si>
+    <t>No consistent SLOs or monitoring for Risk monitoring and trending analysis; outages discovered by users; noisy alerts. 
+Example: On-call lacks actionable alerts.</t>
+  </si>
+  <si>
+    <t>Dashboards exist for Risk monitoring and trending analysis; SLOs drafted but not enforced; triage manual; follow-up inconsistent. 
+Example: No error-budget policy.</t>
+  </si>
+  <si>
+    <t>Analysts follow a trend method: calculate moving averages/seasonality, explain drivers, reference incidents/controls/changes, and propose actions with owners/dates; adverse trends create tracker items. A monthly commentary pack is produced for forums.</t>
+  </si>
+  <si>
+    <t>Qualitative: Risk analysts produce trend commentary that explains movements and drivers and proposes actions; outliers are investigated; links to incidents and controls are explicit. 
+Quantitative: Monthly trend packs on time ≥95%; actions raised per adverse trend; closure P95 ≤30 days. 
+Example: Dashboards/logs show targets met for Risk monitoring and trending analysis; variances generate actions with owners.</t>
+  </si>
+  <si>
+    <t>Reliability engineering for Risk monitoring and trending analysis reduces toil; error-budgets guide decisions; SLO attainment improves. 
+Example: Paging volume down; SLO compliance up.</t>
+  </si>
+  <si>
+    <t>Breach handling unclear; notifications late or inaccurate; evidence not retained. 
+Example: No 72-hour awareness process.</t>
+  </si>
+  <si>
+    <t>Breach procedures drafted; roles trained; some on-time notifications; documentation variable. 
+Example: Near misses not captured.</t>
+  </si>
+  <si>
+    <t>Playbooks link each KRI threshold to actions and escalation (who, when, how), including timer start, comms templates, regulatory triggers (where relevant), and evidence to capture. Overrides require rationale and approval; closure requires verification of effect.</t>
+  </si>
+  <si>
+    <t>Qualitative: Breach playbooks meet statutory content/timelines and are rehearsed; notifications are accurate; evidence and decisions retained. 
+Quantitative: Notification timeliness 100%; post‑breach actions closed to SLO; recurrence of similar cause &lt;5%. 
+Example: Dashboards/logs show targets met for Threshold breach escalation playbooks; variances generate actions with owners.</t>
+  </si>
+  <si>
+    <t>Rehearsed breach playbooks; accurate notifications; evidence retained; themes drive mitigations. 
+Example: Timeliness 100%; similar issues drop.</t>
   </si>
 </sst>
 </file>
@@ -6976,91 +7084,6 @@
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -7145,6 +7168,24 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -7354,6 +7395,73 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7368,135 +7476,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38CE8689-9F1C-43F9-B700-F298F69C440E}" name="Framework" displayName="Framework" ref="A1:H104" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14">
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:H104" xr:uid="{38CE8689-9F1C-43F9-B700-F298F69C440E}">
-    <filterColumn colId="6">
-      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x14">
-          <filters>
-            <x14:filter val="Qualitative: The Alternative workflow and manual processes process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Alternative workflow and manual processes; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Board-approved operational resilience strategy process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Board-approved operational resilience strategy; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Capital and liquidity buffers process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Capital and liquidity buffers; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Comprehensive BIA methodology process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Comprehensive BIA methodology; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Contract management and SLAs process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Contract management and SLAs; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Crisis activation and escalation process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Crisis activation and escalation; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Due diligence and onboarding process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Due diligence and onboarding; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Employee engagement and ownership process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Employee engagement and ownership; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Employee wellbeing programmes process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Employee wellbeing programmes; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Examination and inspection readiness process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Examination and inspection readiness; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Exception and waiver governance process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Exception and waiver governance; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Governance and oversight structure process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Governance and oversight structure; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Important business services register process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Important business services register; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Independent challenge and escalation mechanisms process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Independent challenge and escalation mechanisms; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Information lifecycle management process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Information lifecycle management; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Issue and action tracking workflow process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Issue and action tracking workflow; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Issue remediation and closure process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Issue remediation and closure; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Leadership commitment and messaging process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Leadership commitment and messaging; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Master data and reference architecture process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Master data and reference architecture; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Media and public relations process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Media and public relations; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Operational resilience governance structure process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Operational resilience governance structure; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Post-exercise analysis and improvement process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Post-exercise analysis and improvement; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Predictive risk analytics process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Predictive risk analytics; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Process standardization and optimization process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Process standardization and optimization; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Regulatory feedback integration process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Regulatory feedback integration; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Regulatory horizon scanning process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Regulatory horizon scanning; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Regulatory notification management process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Regulatory notification management; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Regulatory self-assessment processes process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Regulatory self-assessment processes; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Remote work and flexibility process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Remote work and flexibility; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Residual risk rating methodology process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Residual risk rating methodology; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Resilience mindset and behaviors process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Resilience mindset and behaviors; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Security operations and incident response process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Security operations and incident response; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Service level architecture process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Service level architecture; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Simulation and experiential learning process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Simulation and experiential learning; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Single point of failure identification process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Single point of failure identification; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Skills assessment and gap analysis process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Skills assessment and gap analysis; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Supervisory relationship management process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_MI on timeliness/quality of responses; repeat-issue rate trending down; risk-based playbooks for incident notifications._x000a_Pre-reads aligned to tolerance headroom and resilience MI; external feedback loops into policy/controls._x000a_Example: Dashboards/logs show targets met for Supervisory relationship management; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Supply chain risk assessment process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Supply chain risk assessment; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Version control and change management process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Version control and change management; variances generate actions with owners."/>
-            <x14:filter val="Qualitative: The Workforce contingency planning process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Quantitative: KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Workforce contingency planning; variances generate actions with owners."/>
-            <x14:filter val="The Standardized BC plan framework process is executed consistently as designed with clear roles, artefacts and day‑to‑day evidence of control. _x000a_Searchable plan portal; usage/currency analytics; drills validate usability; defects flow to backlog; supplier access tested._x000a_KPIs/KRIs for this process achieved ≥95%; variances trigger timely corrective action; audit issues closed within SLO. _x000a_Example: Dashboards/logs show targets met for Standardized BC plan framework; variances generate actions with owners."/>
-          </filters>
-        </mc:Choice>
-        <mc:Fallback>
-          <customFilters>
-            <customFilter val=""/>
-            <customFilter operator="notEqual" val=" "/>
-          </customFilters>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H104">
-    <sortCondition ref="A2:A104"/>
-    <sortCondition ref="B2:B104"/>
-    <sortCondition ref="C2:C104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38CE8689-9F1C-43F9-B700-F298F69C440E}" name="Framework" displayName="Framework" ref="A1:H106" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
+  <autoFilter ref="A1:H106" xr:uid="{38CE8689-9F1C-43F9-B700-F298F69C440E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H106">
+    <sortCondition ref="A2:A106"/>
+    <sortCondition ref="B2:B106"/>
+    <sortCondition ref="C2:C106"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0093D61F-B69E-457B-A05D-E5B0AB1D0BA3}" name="Dimension"/>
-    <tableColumn id="2" xr3:uid="{0FB31B3F-B70C-4D60-853D-8C2A86F33D4C}" name="Theme" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{975DF045-104A-4165-938B-21FCD45B16AF}" name="Topic" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7F44786E-0AF5-4109-869B-783C590EC47D}" name="1 Initial" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{673A7CEA-C506-47C8-9ECB-024A63A3C957}" name="2 Managed" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{41282D69-C2E8-4889-8192-7EF494BD1B3B}" name="3 Defined" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{5BA7495C-F296-4558-B8E1-A47545ECDD13}" name="4 Quantitatively Managed" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{4C19FB59-0F5E-4F52-8D93-FEC49D806829}" name="5 Optimising" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0FB31B3F-B70C-4D60-853D-8C2A86F33D4C}" name="Theme" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{975DF045-104A-4165-938B-21FCD45B16AF}" name="Topic" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{7F44786E-0AF5-4109-869B-783C590EC47D}" name="1 Initial" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{673A7CEA-C506-47C8-9ECB-024A63A3C957}" name="2 Managed" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{41282D69-C2E8-4889-8192-7EF494BD1B3B}" name="3 Defined" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{5BA7495C-F296-4558-B8E1-A47545ECDD13}" name="4 Quantitatively Managed" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{4C19FB59-0F5E-4F52-8D93-FEC49D806829}" name="5 Optimising" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{643E1880-A5B6-4AB3-82FD-B8E67437DF17}" name="CMMI_definitions" displayName="CMMI_definitions" ref="A1:B6" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{643E1880-A5B6-4AB3-82FD-B8E67437DF17}" name="CMMI_definitions" displayName="CMMI_definitions" ref="A1:B6" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
   <autoFilter ref="A1:B6" xr:uid="{643E1880-A5B6-4AB3-82FD-B8E67437DF17}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3A19EC98-9011-4A57-B752-3199EE2AA661}" name="Level" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{443EFA67-FDDD-4D83-BC75-92A47BB1EDCA}" name="Definition" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{3A19EC98-9011-4A57-B752-3199EE2AA661}" name="Level" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{443EFA67-FDDD-4D83-BC75-92A47BB1EDCA}" name="Definition" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B022752F-B219-4222-9DB2-E8982D75907C}" name="dimension_desc" displayName="dimension_desc" ref="A1:B10" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B022752F-B219-4222-9DB2-E8982D75907C}" name="dimension_desc" displayName="dimension_desc" ref="A1:B10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
   <autoFilter ref="A1:B10" xr:uid="{B022752F-B219-4222-9DB2-E8982D75907C}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F84A265F-5D7B-45AD-8279-8FF81C0F8672}" name="Dimension" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{60EAC33C-0FF5-4068-8DD2-901DAA68762A}" name="Dimension_Description" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{F84A265F-5D7B-45AD-8279-8FF81C0F8672}" name="Dimension" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{60EAC33C-0FF5-4068-8DD2-901DAA68762A}" name="Dimension_Description" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4E66B40B-5A89-438A-BC55-C25A01018498}" name="theme_desc" displayName="theme_desc" ref="D1:E28" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4E66B40B-5A89-438A-BC55-C25A01018498}" name="theme_desc" displayName="theme_desc" ref="D1:E28" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
   <autoFilter ref="D1:E28" xr:uid="{4E66B40B-5A89-438A-BC55-C25A01018498}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2CBFB1F1-70AF-41E1-8963-46393F824366}" name="Theme" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{A4340CD8-0F94-40E6-8C80-D84D85A67C64}" name="Theme_Description" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{2CBFB1F1-70AF-41E1-8963-46393F824366}" name="Theme" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{A4340CD8-0F94-40E6-8C80-D84D85A67C64}" name="Theme_Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5E1C6B87-2747-458C-B3F5-EFCC110AE996}" name="topic_desc" displayName="topic_desc" ref="G1:N104" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
-  <autoFilter ref="G1:N104" xr:uid="{5E1C6B87-2747-458C-B3F5-EFCC110AE996}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5E1C6B87-2747-458C-B3F5-EFCC110AE996}" name="topic_desc" displayName="topic_desc" ref="G1:N106" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="G1:N106" xr:uid="{5E1C6B87-2747-458C-B3F5-EFCC110AE996}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{570AE7C9-317D-4313-93E3-1D765C0EE7B5}" name="Topic" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{9CB8E865-3D67-4610-B58B-5E6220390C74}" name="Topic_Description" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{817CD10B-C459-4229-8C73-49217E3C27F2}" name="Impact (when weak)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{E5C17038-224B-4091-B5D5-012F7816B2F4}" name="Benefits (when strong)" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{762C6A19-BF31-4E6E-9B30-67B40E60FF5B}" name="Basic implementation" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{56AD8473-87CD-4924-BE97-A71C2702154D}" name="Advanced implementation" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5D0BADAF-4F33-4B1F-94B2-1BE8A8DDFFBB}" name="Evidence of effectiveness" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{2D400BA3-AA11-4FD9-9649-F6FD5B1DEA1C}" name="Regulatory pointers" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{570AE7C9-317D-4313-93E3-1D765C0EE7B5}" name="Topic" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{9CB8E865-3D67-4610-B58B-5E6220390C74}" name="Topic_Description" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{817CD10B-C459-4229-8C73-49217E3C27F2}" name="Impact (when weak)" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E5C17038-224B-4091-B5D5-012F7816B2F4}" name="Benefits (when strong)" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{762C6A19-BF31-4E6E-9B30-67B40E60FF5B}" name="Basic implementation" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{56AD8473-87CD-4924-BE97-A71C2702154D}" name="Advanced implementation" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{5D0BADAF-4F33-4B1F-94B2-1BE8A8DDFFBB}" name="Evidence of effectiveness" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{2D400BA3-AA11-4FD9-9649-F6FD5B1DEA1C}" name="Regulatory pointers" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F92EA2F-6518-45D6-8E73-E52F6643E6B4}" name="theme_generic" displayName="theme_generic" ref="A1:G28" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4F92EA2F-6518-45D6-8E73-E52F6643E6B4}" name="theme_generic" displayName="theme_generic" ref="A1:G28" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:G28" xr:uid="{4F92EA2F-6518-45D6-8E73-E52F6643E6B4}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0E1C92DE-7F92-4C27-AF5C-C9BA9951D8D2}" name="Theme"/>
@@ -7512,15 +7564,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4012C250-9782-44B4-874A-ECEDAADCA7EF}" name="Acronyms" displayName="Acronyms" ref="A1:C66" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4012C250-9782-44B4-874A-ECEDAADCA7EF}" name="Acronyms" displayName="Acronyms" ref="A1:C66" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:C66" xr:uid="{4012C250-9782-44B4-874A-ECEDAADCA7EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C66">
     <sortCondition ref="A1:A66"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{64DE9952-5C98-4FAA-B58E-954377CCAEE1}" name="Acronym"/>
-    <tableColumn id="2" xr3:uid="{CCE748DB-BD35-41F6-A6C5-B35F825B4553}" name="Full terminology" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{A87C3444-FD37-4FF7-A298-756975455F8A}" name="Meaning / Why it matters in this framework" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CCE748DB-BD35-41F6-A6C5-B35F825B4553}" name="Full terminology" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{A87C3444-FD37-4FF7-A298-756975455F8A}" name="Meaning / Why it matters in this framework" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7847,10 +7899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7959,7 +8011,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>420</v>
       </c>
@@ -7985,7 +8037,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>420</v>
       </c>
@@ -8037,7 +8089,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>420</v>
       </c>
@@ -8089,7 +8141,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>420</v>
       </c>
@@ -8115,7 +8167,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>420</v>
       </c>
@@ -8167,7 +8219,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>420</v>
       </c>
@@ -8245,7 +8297,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -8297,7 +8349,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -8401,7 +8453,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -8505,7 +8557,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -8557,7 +8609,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -8583,7 +8635,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -8687,7 +8739,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -8765,7 +8817,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -8791,7 +8843,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -8843,7 +8895,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>421</v>
       </c>
@@ -8869,7 +8921,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>421</v>
       </c>
@@ -8895,7 +8947,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>421</v>
       </c>
@@ -8921,7 +8973,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>421</v>
       </c>
@@ -8947,7 +8999,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>421</v>
       </c>
@@ -8976,7 +9028,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>421</v>
       </c>
@@ -9002,7 +9054,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>421</v>
       </c>
@@ -9054,7 +9106,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>421</v>
       </c>
@@ -9106,7 +9158,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -9158,7 +9210,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -9184,7 +9236,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -9210,7 +9262,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -9236,7 +9288,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -9262,7 +9314,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -9288,7 +9340,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -9314,7 +9366,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -9340,7 +9392,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -9366,7 +9418,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -9392,7 +9444,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -9418,7 +9470,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -9444,7 +9496,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -9470,7 +9522,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -9496,7 +9548,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -9574,7 +9626,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -9600,7 +9652,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -9678,7 +9730,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -9782,7 +9834,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -9808,7 +9860,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -9860,7 +9912,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -9886,7 +9938,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -9912,7 +9964,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -9938,7 +9990,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -10068,7 +10120,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -10094,7 +10146,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>13</v>
       </c>
@@ -10120,7 +10172,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>13</v>
       </c>
@@ -10146,7 +10198,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -10172,7 +10224,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>13</v>
       </c>
@@ -10224,7 +10276,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
@@ -10250,7 +10302,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>13</v>
       </c>
@@ -10302,111 +10354,111 @@
         <v>556</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>115</v>
+        <v>1704</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>800</v>
+        <v>1720</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>801</v>
+        <v>1721</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>802</v>
+        <v>1722</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>559</v>
+        <v>1723</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>867</v>
+        <v>1712</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>868</v>
+        <v>1725</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>869</v>
+        <v>1726</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>870</v>
+        <v>1727</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>871</v>
+        <v>1728</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>898</v>
+        <v>115</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>894</v>
+        <v>867</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>803</v>
+        <v>868</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>804</v>
+        <v>869</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>355</v>
+        <v>870</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>560</v>
+        <v>871</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="195" hidden="1" x14ac:dyDescent="0.25">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -10414,25 +10466,25 @@
         <v>37</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>108</v>
+        <v>898</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="210" hidden="1" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -10440,25 +10492,25 @@
         <v>37</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>353</v>
+        <v>807</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -10466,74 +10518,74 @@
         <v>37</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>110</v>
+        <v>894</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="330" hidden="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -10544,25 +10596,25 @@
         <v>38</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="300" hidden="1" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -10570,21 +10622,73 @@
         <v>38</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>818</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="E106" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="F106" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G104" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="H104" s="2" t="s">
+      <c r="H106" s="2" t="s">
         <v>606</v>
       </c>
     </row>
@@ -10668,9 +10772,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N104"/>
+  <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13617,6 +13723,58 @@
       </c>
       <c r="N104" s="2" t="s">
         <v>1564</v>
+      </c>
+    </row>
+    <row r="105" spans="7:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="G105" s="2" t="s">
+        <v>1704</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>1705</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>1706</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>1707</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>1708</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>1709</v>
+      </c>
+      <c r="M105" s="2" t="s">
+        <v>1710</v>
+      </c>
+      <c r="N105" s="2" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="106" spans="7:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="G106" s="2" t="s">
+        <v>1712</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>1713</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>1714</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>1715</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>1716</v>
+      </c>
+      <c r="L106" s="2" t="s">
+        <v>1717</v>
+      </c>
+      <c r="M106" s="2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="N106" s="2" t="s">
+        <v>1719</v>
       </c>
     </row>
   </sheetData>
@@ -14300,7 +14458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>